<commit_message>
Added plots for number of facilities and cumulative investment
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE462E0-F5EB-4660-9A16-FF64B55EA2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0325F-0139-4925-A168-7DA857A9948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="6" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -660,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C400066A-4385-4814-99AE-E0ED2337E160}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1631,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E394EF1B-23F5-4178-BDD5-DE2DF9A8BA3C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1680,7 +1680,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1699,7 +1699,7 @@
         <v>22</v>
       </c>
       <c r="B6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added WTIV plots.  Updated colors
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0325F-0139-4925-A168-7DA857A9948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB69380-DE19-4338-9E1D-753404069CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="6" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="11" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Nexans - Export cable" sheetId="4" r:id="rId8"/>
     <sheet name="Prysmian - Export cable" sheetId="10" r:id="rId9"/>
     <sheet name="Hellenic - Array cable" sheetId="9" r:id="rId10"/>
+    <sheet name="Keppel AmFELS - WTIV" sheetId="11" r:id="rId11"/>
+    <sheet name="Sembcorp - WTIV" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="34">
   <si>
     <t>Factory specifications</t>
   </si>
@@ -137,6 +139,15 @@
   </si>
   <si>
     <t>VA</t>
+  </si>
+  <si>
+    <t>WTIV/year</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Singapore</t>
   </si>
 </sst>
 </file>
@@ -180,9 +191,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +673,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,6 +741,330 @@
       </c>
       <c r="B6">
         <v>2027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A5B857-F2DC-4800-875C-782864066B2E}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194286AF-F140-4E0D-8B09-C499961BC1BC}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>2025</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1631,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E394EF1B-23F5-4178-BDD5-DE2DF9A8BA3C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fiddling with plot colors
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7D6E31-62C5-4951-8E39-0A28B45C2374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AD24A-8EDE-42C2-B6CA-7A4D9EC35D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="12" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A48E9CD-3E39-47A8-B56E-3F49D807C601}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9575DF-18E6-40C8-9E59-D0EA61AD87CB}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2024,7 +2024,7 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -2035,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added spreadsheet for fab port scenarios.  Initial draft of component gantt charts.
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AD24A-8EDE-42C2-B6CA-7A4D9EC35D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5357BACC-8775-4B1C-AEB4-9A1120584BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="7" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9575DF-18E6-40C8-9E59-D0EA61AD87CB}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2310,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CEDFFB-2152-4D3A-9E4D-D879E9700CFD}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated scenario to match Task 4 deliverable
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5357BACC-8775-4B1C-AEB4-9A1120584BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F8631-8510-4F2B-AE0A-9359180C54F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="7" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -1501,168 +1501,6 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>250</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>250</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>150</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FE5F54-BDD9-4AEA-9163-4713DBA3142B}">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1689,7 +1527,169 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
         <v>250</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FE5F54-BDD9-4AEA-9163-4713DBA3142B}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2310,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CEDFFB-2152-4D3A-9E4D-D879E9700CFD}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added ports and vessels to cumulative investment
</commit_message>
<xml_diff>
--- a/library/Announced_factories.xlsx
+++ b/library/Announced_factories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F8631-8510-4F2B-AE0A-9359180C54F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22F8F16-7027-4F6C-893E-64B52CDEA679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="9" activeTab="12" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="EEW - Monopile" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A48E9CD-3E39-47A8-B56E-3F49D807C601}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1662,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FE5F54-BDD9-4AEA-9163-4713DBA3142B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>